<commit_message>
atualização do projeto parents assistance
atualização do plano de projeto +itens+riscos
criação do plano e intereção-E1
correção dos problemas da requisitos
ref campos
erros de especificação

arquitetura
sem UML de classe

prototipo
colocar as telas
</commit_message>
<xml_diff>
--- a/Planejamento/PA_Lista.itens.xlsx
+++ b/Planejamento/PA_Lista.itens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manasses.a.junior\Desktop\Prova Jarley\Planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manasses\Documents\GitHub\ParentsAssistance\Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -117,13 +117,37 @@
   </si>
   <si>
     <t>Manassés</t>
+  </si>
+  <si>
+    <t>Atualizar lista de itens de trabalho</t>
+  </si>
+  <si>
+    <t>Atualizar plano de projeto</t>
+  </si>
+  <si>
+    <t>Atualizar lista de riscos</t>
+  </si>
+  <si>
+    <t>Atualizar plano de iteração</t>
+  </si>
+  <si>
+    <t>Especificação dos casos de uso</t>
+  </si>
+  <si>
+    <t>Projetar em UML os casos de uso</t>
+  </si>
+  <si>
+    <t>Implementação dos casos de uso</t>
+  </si>
+  <si>
+    <t>Criação dos casos de teste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +167,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -173,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -183,17 +213,134 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -201,13 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,13 +362,38 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -244,9 +414,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -284,7 +454,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -356,7 +526,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,388 +700,670 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="16">
         <v>1</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="16">
         <v>2</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>1</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>5</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>1</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="7"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>4</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>2</v>
       </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7">
-        <v>3</v>
-      </c>
-      <c r="H6" s="7">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="G6" s="5">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="7">
-        <v>3</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="G7" s="5">
+        <v>3</v>
+      </c>
+      <c r="H7" s="5">
         <v>4</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="7"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7">
-        <v>3</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="G8" s="5">
+        <v>3</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="7">
-        <v>3</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>6</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>6</v>
       </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>10</v>
       </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>6</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>6</v>
       </c>
-      <c r="H12" s="7">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <v>4</v>
       </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="18">
+        <v>5</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0</v>
+      </c>
+      <c r="H15" s="18">
+        <v>5</v>
+      </c>
+      <c r="I15" s="19"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="18">
+        <v>3</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="18">
+        <v>3</v>
+      </c>
+      <c r="H16" s="18">
+        <v>0</v>
+      </c>
+      <c r="I16" s="19"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="18">
+        <v>4</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0</v>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="18">
+        <v>3</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="19"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="18">
+        <v>3</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="18">
+        <v>3</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0</v>
+      </c>
+      <c r="I19" s="19"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="18">
+        <v>6</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
+      <c r="H20" s="18">
+        <v>5</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="18">
+        <v>10</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
+      <c r="H21" s="18">
+        <v>3</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="18">
+        <v>6</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22" s="18">
+        <v>4</v>
+      </c>
+      <c r="I22" s="19"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="20">
+        <v>4</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0</v>
+      </c>
+      <c r="H23" s="20">
+        <v>10</v>
+      </c>
+      <c r="I23" s="21"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>